<commit_message>
sugar tips and last update of sprints
sugar tips and last update of sprints
</commit_message>
<xml_diff>
--- a/Lap1/sprint.xlsx
+++ b/Lap1/sprint.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farah\Desktop\Health-life-app1\Lap1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mennah\Documents\GitHub\Health-life-app\Lap1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,10 +2051,10 @@
         <v>51</v>
       </c>
       <c r="C59" s="10">
-        <v>43201</v>
+        <v>43193</v>
       </c>
       <c r="D59" s="10">
-        <v>43201</v>
+        <v>43200</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="8" t="s">
@@ -2073,10 +2073,10 @@
         <v>17</v>
       </c>
       <c r="C60" s="10">
-        <v>43201</v>
+        <v>43193</v>
       </c>
       <c r="D60" s="10">
-        <v>43202</v>
+        <v>43194</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>122</v>
@@ -2091,10 +2091,10 @@
         <v>125</v>
       </c>
       <c r="C61" s="10">
-        <v>43202</v>
+        <v>43194</v>
       </c>
       <c r="D61" s="10">
-        <v>43203</v>
+        <v>43195</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>118</v>
@@ -2109,10 +2109,10 @@
         <v>18</v>
       </c>
       <c r="C62" s="10">
-        <v>43203</v>
+        <v>43195</v>
       </c>
       <c r="D62" s="10">
-        <v>43203</v>
+        <v>43195</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>117</v>
@@ -2127,10 +2127,10 @@
         <v>52</v>
       </c>
       <c r="C63" s="10">
-        <v>43203</v>
+        <v>43195</v>
       </c>
       <c r="D63" s="10">
-        <v>43204</v>
+        <v>43196</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>117</v>
@@ -2145,10 +2145,10 @@
         <v>53</v>
       </c>
       <c r="C64" s="10">
-        <v>43204</v>
+        <v>43196</v>
       </c>
       <c r="D64" s="10">
-        <v>43204</v>
+        <v>43196</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>118</v>
@@ -2163,10 +2163,10 @@
         <v>54</v>
       </c>
       <c r="C65" s="10">
-        <v>43204</v>
+        <v>43196</v>
       </c>
       <c r="D65" s="10">
-        <v>43205</v>
+        <v>43197</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>118</v>
@@ -2181,10 +2181,10 @@
         <v>56</v>
       </c>
       <c r="C66" s="10">
-        <v>43205</v>
+        <v>43197</v>
       </c>
       <c r="D66" s="10">
-        <v>43205</v>
+        <v>43197</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="8" t="s">
@@ -2197,10 +2197,10 @@
         <v>59</v>
       </c>
       <c r="C67" s="10">
-        <v>43205</v>
+        <v>43197</v>
       </c>
       <c r="D67" s="10">
-        <v>43206</v>
+        <v>43198</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>121</v>
@@ -2215,10 +2215,10 @@
         <v>57</v>
       </c>
       <c r="C68" s="10">
-        <v>43206</v>
+        <v>43198</v>
       </c>
       <c r="D68" s="10">
-        <v>43206</v>
+        <v>43198</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>119</v>
@@ -2233,10 +2233,10 @@
         <v>58</v>
       </c>
       <c r="C69" s="10">
-        <v>43206</v>
+        <v>43198</v>
       </c>
       <c r="D69" s="10">
-        <v>43207</v>
+        <v>43199</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>120</v>
@@ -2251,10 +2251,10 @@
         <v>55</v>
       </c>
       <c r="C70" s="10">
-        <v>43207</v>
+        <v>43199</v>
       </c>
       <c r="D70" s="10">
-        <v>43207</v>
+        <v>43199</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>119</v>
@@ -2269,10 +2269,10 @@
         <v>60</v>
       </c>
       <c r="C71" s="10">
-        <v>43207</v>
+        <v>43199</v>
       </c>
       <c r="D71" s="10">
-        <v>43207</v>
+        <v>43199</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>122</v>
@@ -2287,10 +2287,10 @@
         <v>61</v>
       </c>
       <c r="C72" s="10">
-        <v>43207</v>
+        <v>43199</v>
       </c>
       <c r="D72" s="10">
-        <v>43207</v>
+        <v>43199</v>
       </c>
       <c r="E72" s="8"/>
       <c r="F72" s="8" t="s">
@@ -2303,10 +2303,10 @@
         <v>62</v>
       </c>
       <c r="C73" s="10">
-        <v>43207</v>
+        <v>43199</v>
       </c>
       <c r="D73" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>121</v>
@@ -2321,10 +2321,10 @@
         <v>63</v>
       </c>
       <c r="C74" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="D74" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>117</v>
@@ -2339,10 +2339,10 @@
         <v>58</v>
       </c>
       <c r="C75" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="D75" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>117</v>
@@ -2357,10 +2357,10 @@
         <v>64</v>
       </c>
       <c r="C76" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="D76" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>120</v>
@@ -2383,10 +2383,10 @@
         <v>65</v>
       </c>
       <c r="C78" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="D78" s="10">
-        <v>43211</v>
+        <v>43203</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="8" t="s">
@@ -2399,10 +2399,10 @@
         <v>17</v>
       </c>
       <c r="C79" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="D79" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>119</v>
@@ -2417,10 +2417,10 @@
         <v>125</v>
       </c>
       <c r="C80" s="10">
-        <v>43208</v>
+        <v>43200</v>
       </c>
       <c r="D80" s="10">
-        <v>43209</v>
+        <v>43201</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>117</v>
@@ -2435,10 +2435,10 @@
         <v>18</v>
       </c>
       <c r="C81" s="10">
-        <v>43209</v>
+        <v>43201</v>
       </c>
       <c r="D81" s="10">
-        <v>43209</v>
+        <v>43201</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>122</v>
@@ -2453,10 +2453,10 @@
         <v>66</v>
       </c>
       <c r="C82" s="10">
-        <v>43209</v>
+        <v>43201</v>
       </c>
       <c r="D82" s="10">
-        <v>43210</v>
+        <v>43202</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>118</v>
@@ -2471,10 +2471,10 @@
         <v>67</v>
       </c>
       <c r="C83" s="10">
-        <v>43210</v>
+        <v>43202</v>
       </c>
       <c r="D83" s="10">
-        <v>43210</v>
+        <v>43202</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>121</v>
@@ -2489,10 +2489,10 @@
         <v>58</v>
       </c>
       <c r="C84" s="10">
-        <v>43210</v>
+        <v>43202</v>
       </c>
       <c r="D84" s="10">
-        <v>43210</v>
+        <v>43202</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>120</v>
@@ -2507,10 +2507,10 @@
         <v>68</v>
       </c>
       <c r="C85" s="10">
-        <v>43210</v>
+        <v>43202</v>
       </c>
       <c r="D85" s="10">
-        <v>43211</v>
+        <v>43203</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>117</v>
@@ -2525,10 +2525,10 @@
         <v>69</v>
       </c>
       <c r="C86" s="10">
-        <v>43211</v>
+        <v>43203</v>
       </c>
       <c r="D86" s="10">
-        <v>43211</v>
+        <v>43203</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>120</v>
@@ -2543,10 +2543,10 @@
         <v>19</v>
       </c>
       <c r="C87" s="10">
-        <v>43211</v>
+        <v>43203</v>
       </c>
       <c r="D87" s="10">
-        <v>43211</v>
+        <v>43203</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>121</v>
@@ -2569,10 +2569,10 @@
         <v>70</v>
       </c>
       <c r="C89" s="10">
-        <v>43211</v>
+        <v>43203</v>
       </c>
       <c r="D89" s="10">
-        <v>43214</v>
+        <v>43206</v>
       </c>
       <c r="E89" s="8"/>
       <c r="F89" s="8" t="s">
@@ -2585,10 +2585,10 @@
         <v>71</v>
       </c>
       <c r="C90" s="10">
-        <v>43211</v>
+        <v>43203</v>
       </c>
       <c r="D90" s="10">
-        <v>43212</v>
+        <v>43204</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>119</v>
@@ -2603,10 +2603,10 @@
         <v>72</v>
       </c>
       <c r="C91" s="10">
-        <v>43212</v>
+        <v>43204</v>
       </c>
       <c r="D91" s="10">
-        <v>43212</v>
+        <v>43204</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>120</v>
@@ -2621,10 +2621,10 @@
         <v>73</v>
       </c>
       <c r="C92" s="10">
-        <v>43212</v>
+        <v>43204</v>
       </c>
       <c r="D92" s="10">
-        <v>43212</v>
+        <v>43204</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>122</v>
@@ -2639,10 +2639,10 @@
         <v>74</v>
       </c>
       <c r="C93" s="10">
-        <v>43213</v>
+        <v>43205</v>
       </c>
       <c r="D93" s="10">
-        <v>43213</v>
+        <v>43205</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>121</v>
@@ -2657,10 +2657,10 @@
         <v>75</v>
       </c>
       <c r="C94" s="10">
-        <v>43213</v>
+        <v>43205</v>
       </c>
       <c r="D94" s="10">
-        <v>43214</v>
+        <v>43206</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>118</v>
@@ -2683,10 +2683,10 @@
         <v>76</v>
       </c>
       <c r="C96" s="10">
-        <v>43214</v>
+        <v>43206</v>
       </c>
       <c r="D96" s="10">
-        <v>43216</v>
+        <v>43208</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>120</v>
@@ -2701,10 +2701,10 @@
         <v>77</v>
       </c>
       <c r="C97" s="10">
-        <v>43215</v>
+        <v>43207</v>
       </c>
       <c r="D97" s="10">
-        <v>43216</v>
+        <v>43208</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>118</v>
@@ -2737,10 +2737,10 @@
         <v>87</v>
       </c>
       <c r="C100" s="10">
-        <v>43218</v>
+        <v>43210</v>
       </c>
       <c r="D100" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="8" t="s">
@@ -2759,10 +2759,10 @@
         <v>17</v>
       </c>
       <c r="C101" s="10">
-        <v>43218</v>
+        <v>43210</v>
       </c>
       <c r="D101" s="10">
-        <v>43218</v>
+        <v>43210</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="8" t="s">
@@ -2775,10 +2775,10 @@
         <v>125</v>
       </c>
       <c r="C102" s="10">
-        <v>43218</v>
+        <v>43210</v>
       </c>
       <c r="D102" s="10">
-        <v>43218</v>
+        <v>43210</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="8" t="s">
@@ -2791,10 +2791,10 @@
         <v>18</v>
       </c>
       <c r="C103" s="10">
-        <v>43218</v>
+        <v>43210</v>
       </c>
       <c r="D103" s="10">
-        <v>43218</v>
+        <v>43210</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="8" t="s">
@@ -2807,10 +2807,10 @@
         <v>20</v>
       </c>
       <c r="C104" s="10">
-        <v>43218</v>
+        <v>43210</v>
       </c>
       <c r="D104" s="10">
-        <v>43219</v>
+        <v>43211</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="8" t="s">
@@ -2823,10 +2823,10 @@
         <v>88</v>
       </c>
       <c r="C105" s="10">
-        <v>43219</v>
+        <v>43211</v>
       </c>
       <c r="D105" s="10">
-        <v>43219</v>
+        <v>43211</v>
       </c>
       <c r="E105" s="8"/>
       <c r="F105" s="8" t="s">
@@ -2839,10 +2839,10 @@
         <v>89</v>
       </c>
       <c r="C106" s="10">
-        <v>43219</v>
+        <v>43211</v>
       </c>
       <c r="D106" s="10">
-        <v>43219</v>
+        <v>43211</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="8" t="s">
@@ -2855,10 +2855,10 @@
         <v>90</v>
       </c>
       <c r="C107" s="10">
-        <v>43219</v>
+        <v>43211</v>
       </c>
       <c r="D107" s="10">
-        <v>43219</v>
+        <v>43211</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="8" t="s">
@@ -2871,10 +2871,10 @@
         <v>91</v>
       </c>
       <c r="C108" s="10">
-        <v>43219</v>
+        <v>43211</v>
       </c>
       <c r="D108" s="10">
-        <v>43220</v>
+        <v>43212</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="8" t="s">
@@ -2887,10 +2887,10 @@
         <v>92</v>
       </c>
       <c r="C109" s="10">
-        <v>43220</v>
+        <v>43212</v>
       </c>
       <c r="D109" s="10">
-        <v>43220</v>
+        <v>43212</v>
       </c>
       <c r="E109" s="8"/>
       <c r="F109" s="8" t="s">
@@ -2903,10 +2903,10 @@
         <v>93</v>
       </c>
       <c r="C110" s="10">
-        <v>43220</v>
+        <v>43212</v>
       </c>
       <c r="D110" s="10">
-        <v>43220</v>
+        <v>43212</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="8" t="s">
@@ -2919,10 +2919,10 @@
         <v>94</v>
       </c>
       <c r="C111" s="10">
-        <v>43220</v>
+        <v>43212</v>
       </c>
       <c r="D111" s="10">
-        <v>43221</v>
+        <v>43213</v>
       </c>
       <c r="E111" s="8"/>
       <c r="F111" s="8" t="s">
@@ -2935,10 +2935,10 @@
         <v>95</v>
       </c>
       <c r="C112" s="10">
-        <v>43221</v>
+        <v>43213</v>
       </c>
       <c r="D112" s="10">
-        <v>43221</v>
+        <v>43213</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="8" t="s">
@@ -2951,10 +2951,10 @@
         <v>96</v>
       </c>
       <c r="C113" s="10">
-        <v>43221</v>
+        <v>43213</v>
       </c>
       <c r="D113" s="10">
-        <v>43222</v>
+        <v>43214</v>
       </c>
       <c r="E113" s="8"/>
       <c r="F113" s="8" t="s">
@@ -2967,10 +2967,10 @@
         <v>97</v>
       </c>
       <c r="C114" s="10">
-        <v>43222</v>
+        <v>43214</v>
       </c>
       <c r="D114" s="10">
-        <v>43222</v>
+        <v>43214</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="8" t="s">
@@ -2983,10 +2983,10 @@
         <v>98</v>
       </c>
       <c r="C115" s="10">
-        <v>43222</v>
+        <v>43214</v>
       </c>
       <c r="D115" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="E115" s="8"/>
       <c r="F115" s="8" t="s">
@@ -3007,10 +3007,10 @@
         <v>99</v>
       </c>
       <c r="C117" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="D117" s="10">
-        <v>43228</v>
+        <v>43220</v>
       </c>
       <c r="E117" s="8"/>
       <c r="F117" s="8" t="s">
@@ -3023,10 +3023,10 @@
         <v>17</v>
       </c>
       <c r="C118" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="D118" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="E118" s="8"/>
       <c r="F118" s="8" t="s">
@@ -3039,10 +3039,10 @@
         <v>125</v>
       </c>
       <c r="C119" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="D119" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="E119" s="8"/>
       <c r="F119" s="8" t="s">
@@ -3055,10 +3055,10 @@
         <v>18</v>
       </c>
       <c r="C120" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="D120" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="E120" s="8"/>
       <c r="F120" s="8" t="s">
@@ -3071,10 +3071,10 @@
         <v>20</v>
       </c>
       <c r="C121" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="D121" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="E121" s="8"/>
       <c r="F121" s="8" t="s">
@@ -3087,10 +3087,10 @@
         <v>100</v>
       </c>
       <c r="C122" s="10">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="D122" s="10">
-        <v>43224</v>
+        <v>43216</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="8" t="s">
@@ -3103,10 +3103,10 @@
         <v>101</v>
       </c>
       <c r="C123" s="10">
-        <v>43224</v>
+        <v>43216</v>
       </c>
       <c r="D123" s="10">
-        <v>43224</v>
+        <v>43216</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="8" t="s">
@@ -3119,10 +3119,10 @@
         <v>102</v>
       </c>
       <c r="C124" s="10">
-        <v>43224</v>
+        <v>43216</v>
       </c>
       <c r="D124" s="10">
-        <v>43224</v>
+        <v>43216</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="8" t="s">
@@ -3135,10 +3135,10 @@
         <v>103</v>
       </c>
       <c r="C125" s="10">
-        <v>43224</v>
+        <v>43216</v>
       </c>
       <c r="D125" s="10">
-        <v>43225</v>
+        <v>43217</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="8" t="s">
@@ -3151,10 +3151,10 @@
         <v>104</v>
       </c>
       <c r="C126" s="10">
-        <v>43225</v>
+        <v>43217</v>
       </c>
       <c r="D126" s="10">
-        <v>43225</v>
+        <v>43217</v>
       </c>
       <c r="E126" s="8"/>
       <c r="F126" s="8" t="s">
@@ -3167,10 +3167,10 @@
         <v>105</v>
       </c>
       <c r="C127" s="10">
-        <v>43225</v>
+        <v>43217</v>
       </c>
       <c r="D127" s="10">
-        <v>43226</v>
+        <v>43218</v>
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="8" t="s">
@@ -3183,10 +3183,10 @@
         <v>106</v>
       </c>
       <c r="C128" s="10">
-        <v>43226</v>
+        <v>43218</v>
       </c>
       <c r="D128" s="10">
-        <v>43226</v>
+        <v>43218</v>
       </c>
       <c r="E128" s="8"/>
       <c r="F128" s="8" t="s">
@@ -3199,10 +3199,10 @@
         <v>107</v>
       </c>
       <c r="C129" s="10">
-        <v>43226</v>
+        <v>43218</v>
       </c>
       <c r="D129" s="10">
-        <v>43227</v>
+        <v>43219</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="8" t="s">
@@ -3215,10 +3215,10 @@
         <v>108</v>
       </c>
       <c r="C130" s="10">
-        <v>43227</v>
+        <v>43219</v>
       </c>
       <c r="D130" s="10">
-        <v>43227</v>
+        <v>43219</v>
       </c>
       <c r="E130" s="8"/>
       <c r="F130" s="8" t="s">
@@ -3231,10 +3231,10 @@
         <v>109</v>
       </c>
       <c r="C131" s="10">
-        <v>43227</v>
+        <v>43219</v>
       </c>
       <c r="D131" s="10">
-        <v>43227</v>
+        <v>43219</v>
       </c>
       <c r="E131" s="8"/>
       <c r="F131" s="8" t="s">
@@ -3247,10 +3247,10 @@
         <v>110</v>
       </c>
       <c r="C132" s="10">
-        <v>43227</v>
+        <v>43219</v>
       </c>
       <c r="D132" s="10">
-        <v>43228</v>
+        <v>43220</v>
       </c>
       <c r="E132" s="8"/>
       <c r="F132" s="8" t="s">
@@ -3271,10 +3271,10 @@
         <v>64</v>
       </c>
       <c r="C134" s="10">
-        <v>43228</v>
+        <v>43220</v>
       </c>
       <c r="D134" s="10">
-        <v>43228</v>
+        <v>43220</v>
       </c>
       <c r="E134" s="8"/>
       <c r="F134" s="8" t="s">

</xml_diff>